<commit_message>
updated the readme file and runned the current code to the test images
</commit_message>
<xml_diff>
--- a/results/sentiment_analysis_results.xlsx
+++ b/results/sentiment_analysis_results.xlsx
@@ -425,7 +425,7 @@
     <col width="477" customWidth="1" min="2" max="2"/>
     <col width="467" customWidth="1" min="3" max="3"/>
     <col width="16" customWidth="1" min="4" max="4"/>
-    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="82" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
     <col width="19" customWidth="1" min="7" max="7"/>
     <col width="12" customWidth="1" min="8" max="8"/>
@@ -496,22 +496,22 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Error generating caption</t>
+          <t>a man in a white shirt and black pants stands at a podium with a microphone</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>70.09%</t>
+          <t>50.0%</t>
         </is>
       </c>
     </row>
@@ -538,22 +538,22 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Error generating caption</t>
+          <t>a group of people posing for a photo</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>70.09%</t>
+          <t>50.0%</t>
         </is>
       </c>
     </row>
@@ -580,22 +580,22 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Error generating caption</t>
+          <t>a man in a yellow shirt is holding a microphone</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>52.03%</t>
+          <t>68.06%</t>
         </is>
       </c>
     </row>
@@ -622,22 +622,22 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Error generating caption</t>
+          <t>obama and dute</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>70.09%</t>
+          <t>50.0%</t>
         </is>
       </c>
     </row>
@@ -664,22 +664,22 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Error generating caption</t>
+          <t>person giving a speech on stage</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>70.09%</t>
+          <t>67.0%</t>
         </is>
       </c>
     </row>
@@ -706,22 +706,22 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Error generating caption</t>
+          <t>a woman in a red jacket and glasses speaking into a microphone</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>70.09%</t>
+          <t>50.0%</t>
         </is>
       </c>
     </row>
@@ -748,12 +748,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Error generating caption</t>
+          <t>a man in a white shirt and a hat with his head in his hands, with the words what</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -763,7 +763,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>58.73%</t>
+          <t>100%</t>
         </is>
       </c>
     </row>
@@ -790,7 +790,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Error generating caption</t>
+          <t>a man in a white shirt is crying and holding his head</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -805,7 +805,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>70.09%</t>
+          <t>73.84%</t>
         </is>
       </c>
     </row>
@@ -832,12 +832,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Error generating caption</t>
+          <t>two men in suits standing next to each other men</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -874,22 +874,22 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Error generating caption</t>
+          <t>a group of people riding in a boat down a flooded street</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>Negative</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Negative</t>
-        </is>
-      </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>74.97%</t>
         </is>
       </c>
     </row>

</xml_diff>